<commit_message>
Thermometry plots for comparing diff final setpoints
</commit_message>
<xml_diff>
--- a/phase_shift_scanlist.xlsx
+++ b/phase_shift_scanlist.xlsx
@@ -452,13 +452,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>43.19493510534897</v>
+        <v>43.25546567444445</v>
       </c>
       <c r="B2" t="n">
-        <v>4.027764894651033</v>
+        <v>3.967234325555555</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
         <v>0.76</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>43</v>
+        <v>43.21102123</v>
       </c>
       <c r="B3" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01167877</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
         <v>0.76</v>
@@ -486,13 +486,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>43.26501053876748</v>
+        <v>43</v>
       </c>
       <c r="B4" t="n">
-        <v>3.957689461232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0.76</v>
@@ -503,13 +503,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>43.24435456333334</v>
+        <v>43.28300697502331</v>
       </c>
       <c r="B5" t="n">
-        <v>3.978345436666666</v>
+        <v>3.939693024976697</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
         <v>0.76</v>
@@ -520,13 +520,13 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>43.21102123</v>
+        <v>43.23246939620138</v>
       </c>
       <c r="B6" t="n">
-        <v>4.01167877</v>
+        <v>3.990230603798622</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
         <v>0.76</v>
@@ -537,13 +537,13 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>43.22710735465104</v>
+        <v>43</v>
       </c>
       <c r="B7" t="n">
-        <v>3.995592645348967</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0.76</v>
@@ -554,13 +554,13 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>43</v>
+        <v>43.1390354849767</v>
       </c>
       <c r="B8" t="n">
-        <v>4.222700000000003</v>
+        <v>4.083664515023302</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
         <v>0.76</v>
@@ -571,13 +571,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>43.17768789666667</v>
+        <v>43</v>
       </c>
       <c r="B9" t="n">
-        <v>4.045012103333333</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0.76</v>
@@ -588,13 +588,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>43</v>
+        <v>43.16657678555556</v>
       </c>
       <c r="B10" t="n">
-        <v>4.222700000000003</v>
+        <v>4.056123214444444</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
         <v>0.76</v>
@@ -605,13 +605,13 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>43.15703192123253</v>
+        <v>43.18957306379863</v>
       </c>
       <c r="B11" t="n">
-        <v>4.065668078767477</v>
+        <v>4.033126936201377</v>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" t="n">
         <v>0.76</v>
@@ -622,13 +622,13 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>43.19493510534897</v>
+        <v>43.25546567444445</v>
       </c>
       <c r="B12" t="n">
-        <v>4.027764894651033</v>
+        <v>3.967234325555555</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>0.76</v>
@@ -639,13 +639,13 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>43</v>
+        <v>43.21102123</v>
       </c>
       <c r="B13" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01167877</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
         <v>0.76</v>
@@ -656,13 +656,13 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>43.26501053876748</v>
+        <v>43</v>
       </c>
       <c r="B14" t="n">
-        <v>3.957689461232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>0.76</v>
@@ -673,13 +673,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>43.24435456333334</v>
+        <v>43.28300697502331</v>
       </c>
       <c r="B15" t="n">
-        <v>3.978345436666666</v>
+        <v>3.939693024976697</v>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
         <v>0.76</v>
@@ -690,13 +690,13 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>43.21102123</v>
+        <v>43.23246939620138</v>
       </c>
       <c r="B16" t="n">
-        <v>4.01167877</v>
+        <v>3.990230603798622</v>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" t="n">
         <v>0.76</v>
@@ -707,13 +707,13 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>43.22710735465104</v>
+        <v>43</v>
       </c>
       <c r="B17" t="n">
-        <v>3.995592645348967</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0.76</v>
@@ -724,13 +724,13 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>43</v>
+        <v>43.1390354849767</v>
       </c>
       <c r="B18" t="n">
-        <v>4.222700000000003</v>
+        <v>4.083664515023302</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D18" t="n">
         <v>0.76</v>
@@ -741,13 +741,13 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>43.17768789666667</v>
+        <v>43</v>
       </c>
       <c r="B19" t="n">
-        <v>4.045012103333333</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0.76</v>
@@ -758,13 +758,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>43</v>
+        <v>43.16657678555556</v>
       </c>
       <c r="B20" t="n">
-        <v>4.222700000000003</v>
+        <v>4.056123214444444</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D20" t="n">
         <v>0.76</v>
@@ -775,13 +775,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>43.15703192123253</v>
+        <v>43.18957306379863</v>
       </c>
       <c r="B21" t="n">
-        <v>4.065668078767477</v>
+        <v>4.033126936201377</v>
       </c>
       <c r="C21" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21" t="n">
         <v>0.76</v>
@@ -792,13 +792,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>43.16161818489488</v>
+        <v>43.21560749366236</v>
       </c>
       <c r="B22" t="n">
-        <v>4.061081815105119</v>
+        <v>4.007092506337642</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" t="n">
         <v>0.75</v>
@@ -809,13 +809,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>43.23169361831339</v>
+        <v>43.26005193810681</v>
       </c>
       <c r="B23" t="n">
-        <v>3.991006381686609</v>
+        <v>3.962648061893198</v>
       </c>
       <c r="C23" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
         <v>0.75</v>
@@ -826,13 +826,13 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>43</v>
+        <v>43.19415932746098</v>
       </c>
       <c r="B24" t="n">
-        <v>4.222700000000003</v>
+        <v>4.02854067253902</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D24" t="n">
         <v>0.75</v>
@@ -843,13 +843,13 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>43</v>
+        <v>43.17116304921792</v>
       </c>
       <c r="B25" t="n">
-        <v>4.222700000000003</v>
+        <v>4.051536950782086</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D25" t="n">
         <v>0.75</v>
@@ -860,13 +860,13 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>43.21560749366236</v>
+        <v>43.14362174863906</v>
       </c>
       <c r="B26" t="n">
-        <v>4.007092506337642</v>
+        <v>4.079078251360944</v>
       </c>
       <c r="C26" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D26" t="n">
         <v>0.75</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>43.19952136901133</v>
+        <v>43</v>
       </c>
       <c r="B27" t="n">
-        <v>4.023178630988675</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>0.75</v>
@@ -894,13 +894,13 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>43.26959680242984</v>
+        <v>43</v>
       </c>
       <c r="B28" t="n">
-        <v>3.953103197570165</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C28" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0.75</v>
@@ -911,13 +911,13 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>43.24894082699569</v>
+        <v>43.28759323868567</v>
       </c>
       <c r="B29" t="n">
-        <v>3.973759173004309</v>
+        <v>3.93510676131434</v>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D29" t="n">
         <v>0.75</v>
@@ -945,13 +945,13 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>43.18227416032903</v>
+        <v>43.23705565986374</v>
       </c>
       <c r="B31" t="n">
-        <v>4.040425839670975</v>
+        <v>3.985644340136265</v>
       </c>
       <c r="C31" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D31" t="n">
         <v>0.75</v>
@@ -962,13 +962,13 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>43.16161818489488</v>
+        <v>43.21560749366236</v>
       </c>
       <c r="B32" t="n">
-        <v>4.061081815105119</v>
+        <v>4.007092506337642</v>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D32" t="n">
         <v>0.75</v>
@@ -979,13 +979,13 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>43.23169361831339</v>
+        <v>43.26005193810681</v>
       </c>
       <c r="B33" t="n">
-        <v>3.991006381686609</v>
+        <v>3.962648061893198</v>
       </c>
       <c r="C33" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D33" t="n">
         <v>0.75</v>
@@ -996,13 +996,13 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>43</v>
+        <v>43.19415932746098</v>
       </c>
       <c r="B34" t="n">
-        <v>4.222700000000003</v>
+        <v>4.02854067253902</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D34" t="n">
         <v>0.75</v>
@@ -1013,13 +1013,13 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>43</v>
+        <v>43.17116304921792</v>
       </c>
       <c r="B35" t="n">
-        <v>4.222700000000003</v>
+        <v>4.051536950782086</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D35" t="n">
         <v>0.75</v>
@@ -1030,13 +1030,13 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>43.21560749366236</v>
+        <v>43.14362174863906</v>
       </c>
       <c r="B36" t="n">
-        <v>4.007092506337642</v>
+        <v>4.079078251360944</v>
       </c>
       <c r="C36" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D36" t="n">
         <v>0.75</v>
@@ -1047,13 +1047,13 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>43.19952136901133</v>
+        <v>43</v>
       </c>
       <c r="B37" t="n">
-        <v>4.023178630988675</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0.75</v>
@@ -1064,13 +1064,13 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>43.26959680242984</v>
+        <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>3.953103197570165</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C38" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0.75</v>
@@ -1081,13 +1081,13 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>43.24894082699569</v>
+        <v>43.28759323868567</v>
       </c>
       <c r="B39" t="n">
-        <v>3.973759173004309</v>
+        <v>3.93510676131434</v>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D39" t="n">
         <v>0.75</v>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>43.18227416032903</v>
+        <v>43.23705565986374</v>
       </c>
       <c r="B41" t="n">
-        <v>4.040425839670975</v>
+        <v>3.985644340136265</v>
       </c>
       <c r="C41" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D41" t="n">
         <v>0.75</v>
@@ -1132,13 +1132,13 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>43.17388377832302</v>
+        <v>43.29985883211381</v>
       </c>
       <c r="B42" t="n">
-        <v>4.048816221676979</v>
+        <v>3.922841167886201</v>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D42" t="n">
         <v>0.74</v>
@@ -1149,13 +1149,13 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>43.21178696243947</v>
+        <v>43.27231753153495</v>
       </c>
       <c r="B43" t="n">
-        <v>4.010913037560536</v>
+        <v>3.950382468465059</v>
       </c>
       <c r="C43" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D43" t="n">
         <v>0.74</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43.19453975375717</v>
+        <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>4.028160246242837</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C44" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0.74</v>
@@ -1183,13 +1183,13 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>43</v>
+        <v>43.20642492088912</v>
       </c>
       <c r="B45" t="n">
-        <v>4.222700000000003</v>
+        <v>4.016275079110881</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D45" t="n">
         <v>0.74</v>
@@ -1200,13 +1200,13 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>43.24395921174153</v>
+        <v>43</v>
       </c>
       <c r="B46" t="n">
-        <v>3.97874078825847</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C46" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0.74</v>
@@ -1217,13 +1217,13 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>43.28186239585798</v>
+        <v>43</v>
       </c>
       <c r="B47" t="n">
-        <v>3.940837604142026</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C47" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>0.74</v>
@@ -1234,13 +1234,13 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>43.2278730870905</v>
+        <v>43.18342864264606</v>
       </c>
       <c r="B48" t="n">
-        <v>3.994826912909503</v>
+        <v>4.039271357353948</v>
       </c>
       <c r="C48" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D48" t="n">
         <v>0.74</v>
@@ -1251,13 +1251,13 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>43</v>
+        <v>43.24932125329187</v>
       </c>
       <c r="B49" t="n">
-        <v>4.222700000000003</v>
+        <v>3.973378746708125</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D49" t="n">
         <v>0.74</v>
@@ -1268,13 +1268,13 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>43.26120642042383</v>
+        <v>43.1558873420672</v>
       </c>
       <c r="B50" t="n">
-        <v>3.96149357957617</v>
+        <v>4.066812657932806</v>
       </c>
       <c r="C50" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D50" t="n">
         <v>0.74</v>
@@ -1285,13 +1285,13 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>43</v>
+        <v>43.2278730870905</v>
       </c>
       <c r="B51" t="n">
-        <v>4.222700000000003</v>
+        <v>3.994826912909503</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D51" t="n">
         <v>0.74</v>
@@ -1302,13 +1302,13 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>43.17388377832302</v>
+        <v>43.29985883211381</v>
       </c>
       <c r="B52" t="n">
-        <v>4.048816221676979</v>
+        <v>3.922841167886201</v>
       </c>
       <c r="C52" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
         <v>0.74</v>
@@ -1319,13 +1319,13 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>43.21178696243947</v>
+        <v>43.27231753153495</v>
       </c>
       <c r="B53" t="n">
-        <v>4.010913037560536</v>
+        <v>3.950382468465059</v>
       </c>
       <c r="C53" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D53" t="n">
         <v>0.74</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>43.19453975375717</v>
+        <v>43</v>
       </c>
       <c r="B54" t="n">
-        <v>4.028160246242837</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C54" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
         <v>0.74</v>
@@ -1353,13 +1353,13 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>43</v>
+        <v>43.20642492088912</v>
       </c>
       <c r="B55" t="n">
-        <v>4.222700000000003</v>
+        <v>4.016275079110881</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D55" t="n">
         <v>0.74</v>
@@ -1370,13 +1370,13 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>43.24395921174153</v>
+        <v>43</v>
       </c>
       <c r="B56" t="n">
-        <v>3.97874078825847</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C56" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
         <v>0.74</v>
@@ -1387,13 +1387,13 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>43.28186239585798</v>
+        <v>43</v>
       </c>
       <c r="B57" t="n">
-        <v>3.940837604142026</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C57" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0.74</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>43.2278730870905</v>
+        <v>43.18342864264606</v>
       </c>
       <c r="B58" t="n">
-        <v>3.994826912909503</v>
+        <v>4.039271357353948</v>
       </c>
       <c r="C58" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D58" t="n">
         <v>0.74</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>43</v>
+        <v>43.24932125329187</v>
       </c>
       <c r="B59" t="n">
-        <v>4.222700000000003</v>
+        <v>3.973378746708125</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D59" t="n">
         <v>0.74</v>
@@ -1438,13 +1438,13 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>43.26120642042383</v>
+        <v>43.1558873420672</v>
       </c>
       <c r="B60" t="n">
-        <v>3.96149357957617</v>
+        <v>4.066812657932806</v>
       </c>
       <c r="C60" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D60" t="n">
         <v>0.74</v>
@@ -1455,13 +1455,13 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>43</v>
+        <v>43.2278730870905</v>
       </c>
       <c r="B61" t="n">
-        <v>4.222700000000003</v>
+        <v>3.994826912909503</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D61" t="n">
         <v>0.74</v>
@@ -1472,13 +1472,13 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>43</v>
+        <v>43.22168480428568</v>
       </c>
       <c r="B62" t="n">
-        <v>4.222700000000003</v>
+        <v>4.001015195714325</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D62" t="n">
         <v>0.73</v>
@@ -1489,13 +1489,13 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>43</v>
+        <v>43.24313297048705</v>
       </c>
       <c r="B63" t="n">
-        <v>4.222700000000003</v>
+        <v>3.979567029512947</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D63" t="n">
         <v>0.73</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>43.25921909513809</v>
+        <v>43</v>
       </c>
       <c r="B64" t="n">
-        <v>3.963480904861914</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C64" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
         <v>0.73</v>
@@ -1523,13 +1523,13 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>43.22704684583602</v>
+        <v>43.31511871551036</v>
       </c>
       <c r="B65" t="n">
-        <v>3.99565315416398</v>
+        <v>3.907581284489645</v>
       </c>
       <c r="C65" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D65" t="n">
         <v>0.73</v>
@@ -1540,13 +1540,13 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>43.24313297048705</v>
+        <v>43.17114722546376</v>
       </c>
       <c r="B66" t="n">
-        <v>3.979567029512947</v>
+        <v>4.051552774536249</v>
       </c>
       <c r="C66" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D66" t="n">
         <v>0.73</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>43.18914366171958</v>
+        <v>43.26458113668843</v>
       </c>
       <c r="B67" t="n">
-        <v>4.033556338280424</v>
+        <v>3.95811886331157</v>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D67" t="n">
         <v>0.73</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>43.27646630382039</v>
+        <v>43.2875774149315</v>
       </c>
       <c r="B68" t="n">
-        <v>3.946233696179614</v>
+        <v>3.935122585068503</v>
       </c>
       <c r="C68" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D68" t="n">
         <v>0.73</v>
@@ -1591,13 +1591,13 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>43.29712227925453</v>
+        <v>43</v>
       </c>
       <c r="B69" t="n">
-        <v>3.92557772074547</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C69" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
         <v>0.73</v>
@@ -1608,13 +1608,13 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>43</v>
+        <v>43.19868852604261</v>
       </c>
       <c r="B70" t="n">
-        <v>4.222700000000003</v>
+        <v>4.024011473957391</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D70" t="n">
         <v>0.73</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>43.20979963715372</v>
+        <v>43</v>
       </c>
       <c r="B71" t="n">
-        <v>4.01290036284628</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
         <v>0.73</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>43</v>
+        <v>43.22168480428568</v>
       </c>
       <c r="B72" t="n">
-        <v>4.222700000000003</v>
+        <v>4.001015195714325</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D72" t="n">
         <v>0.73</v>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>43</v>
+        <v>43.24313297048705</v>
       </c>
       <c r="B73" t="n">
-        <v>4.222700000000003</v>
+        <v>3.979567029512947</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D73" t="n">
         <v>0.73</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>43.25921909513809</v>
+        <v>43</v>
       </c>
       <c r="B74" t="n">
-        <v>3.963480904861914</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C74" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0.73</v>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>43.22704684583602</v>
+        <v>43.31511871551036</v>
       </c>
       <c r="B75" t="n">
-        <v>3.99565315416398</v>
+        <v>3.907581284489645</v>
       </c>
       <c r="C75" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D75" t="n">
         <v>0.73</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>43.24313297048705</v>
+        <v>43.17114722546376</v>
       </c>
       <c r="B76" t="n">
-        <v>3.979567029512947</v>
+        <v>4.051552774536249</v>
       </c>
       <c r="C76" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D76" t="n">
         <v>0.73</v>
@@ -1727,13 +1727,13 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>43.18914366171958</v>
+        <v>43.26458113668843</v>
       </c>
       <c r="B77" t="n">
-        <v>4.033556338280424</v>
+        <v>3.95811886331157</v>
       </c>
       <c r="C77" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D77" t="n">
         <v>0.73</v>
@@ -1744,13 +1744,13 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>43.27646630382039</v>
+        <v>43.2875774149315</v>
       </c>
       <c r="B78" t="n">
-        <v>3.946233696179614</v>
+        <v>3.935122585068503</v>
       </c>
       <c r="C78" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D78" t="n">
         <v>0.73</v>
@@ -1761,13 +1761,13 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>43.29712227925453</v>
+        <v>43</v>
       </c>
       <c r="B79" t="n">
-        <v>3.92557772074547</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C79" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
         <v>0.73</v>
@@ -1778,13 +1778,13 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>43</v>
+        <v>43.19868852604261</v>
       </c>
       <c r="B80" t="n">
-        <v>4.222700000000003</v>
+        <v>4.024011473957391</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D80" t="n">
         <v>0.73</v>
@@ -1795,13 +1795,13 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>43.20979963715372</v>
+        <v>43</v>
       </c>
       <c r="B81" t="n">
-        <v>4.01290036284628</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C81" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
         <v>0.73</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>43.22222505372558</v>
+        <v>43.30000283150336</v>
       </c>
       <c r="B82" t="n">
-        <v>4.000474946274419</v>
+        <v>3.922697168496642</v>
       </c>
       <c r="C82" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
         <v>0.72</v>
@@ -1829,13 +1829,13 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>43</v>
+        <v>43.25555838705892</v>
       </c>
       <c r="B83" t="n">
-        <v>4.222700000000003</v>
+        <v>3.967141612941086</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D83" t="n">
         <v>0.72</v>
@@ -1846,13 +1846,13 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>43.20156907829144</v>
+        <v>43.23411022085754</v>
       </c>
       <c r="B84" t="n">
-        <v>4.021130921708563</v>
+        <v>3.988589779142464</v>
       </c>
       <c r="C84" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D84" t="n">
         <v>0.72</v>
@@ -1863,13 +1863,13 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>43</v>
+        <v>43.21111394261447</v>
       </c>
       <c r="B85" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01158605738553</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D85" t="n">
         <v>0.72</v>
@@ -1880,13 +1880,13 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>43.27164451170995</v>
+        <v>43.32754413208222</v>
       </c>
       <c r="B86" t="n">
-        <v>3.951055488290053</v>
+        <v>3.895155867917784</v>
       </c>
       <c r="C86" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D86" t="n">
         <v>0.72</v>
@@ -1897,13 +1897,13 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>43.3095476958264</v>
+        <v>43</v>
       </c>
       <c r="B87" t="n">
-        <v>3.913152304173609</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C87" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
         <v>0.72</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>43.28889172039225</v>
+        <v>43.18357264203561</v>
       </c>
       <c r="B88" t="n">
-        <v>3.933808279607753</v>
+        <v>4.039127357964388</v>
       </c>
       <c r="C88" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D88" t="n">
         <v>0.72</v>
@@ -1931,13 +1931,13 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>43.23947226240789</v>
+        <v>43.27700655326029</v>
       </c>
       <c r="B89" t="n">
-        <v>3.983227737592119</v>
+        <v>3.945693446739709</v>
       </c>
       <c r="C89" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D89" t="n">
         <v>0.72</v>
@@ -1965,13 +1965,13 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>43.25555838705892</v>
+        <v>43</v>
       </c>
       <c r="B91" t="n">
-        <v>3.967141612941086</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C91" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
         <v>0.72</v>
@@ -1982,13 +1982,13 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>43.22222505372558</v>
+        <v>43.30000283150336</v>
       </c>
       <c r="B92" t="n">
-        <v>4.000474946274419</v>
+        <v>3.922697168496642</v>
       </c>
       <c r="C92" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
         <v>0.72</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>43</v>
+        <v>43.25555838705892</v>
       </c>
       <c r="B93" t="n">
-        <v>4.222700000000003</v>
+        <v>3.967141612941086</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D93" t="n">
         <v>0.72</v>
@@ -2016,13 +2016,13 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>43.20156907829144</v>
+        <v>43.23411022085754</v>
       </c>
       <c r="B94" t="n">
-        <v>4.021130921708563</v>
+        <v>3.988589779142464</v>
       </c>
       <c r="C94" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D94" t="n">
         <v>0.72</v>
@@ -2033,13 +2033,13 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>43</v>
+        <v>43.21111394261447</v>
       </c>
       <c r="B95" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01158605738553</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D95" t="n">
         <v>0.72</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>43.27164451170995</v>
+        <v>43.32754413208222</v>
       </c>
       <c r="B96" t="n">
-        <v>3.951055488290053</v>
+        <v>3.895155867917784</v>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D96" t="n">
         <v>0.72</v>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>43.3095476958264</v>
+        <v>43</v>
       </c>
       <c r="B97" t="n">
-        <v>3.913152304173609</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C97" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
         <v>0.72</v>
@@ -2084,13 +2084,13 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>43.28889172039225</v>
+        <v>43.18357264203561</v>
       </c>
       <c r="B98" t="n">
-        <v>3.933808279607753</v>
+        <v>4.039127357964388</v>
       </c>
       <c r="C98" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D98" t="n">
         <v>0.72</v>
@@ -2101,13 +2101,13 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>43.23947226240789</v>
+        <v>43.27700655326029</v>
       </c>
       <c r="B99" t="n">
-        <v>3.983227737592119</v>
+        <v>3.945693446739709</v>
       </c>
       <c r="C99" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D99" t="n">
         <v>0.72</v>
@@ -2135,13 +2135,13 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>43.25555838705892</v>
+        <v>43</v>
       </c>
       <c r="B101" t="n">
-        <v>3.967141612941086</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C101" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
         <v>0.72</v>
@@ -2152,13 +2152,13 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>43.26040325</v>
+        <v>43</v>
       </c>
       <c r="B102" t="n">
-        <v>3.96229675</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C102" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
         <v>0.71</v>
@@ -2169,13 +2169,13 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>43.31439255876748</v>
+        <v>43</v>
       </c>
       <c r="B103" t="n">
-        <v>3.908307441232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C103" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
         <v>0.71</v>
@@ -2186,13 +2186,13 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>43</v>
+        <v>43.21595880555556</v>
       </c>
       <c r="B104" t="n">
-        <v>4.222700000000003</v>
+        <v>4.006741194444444</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D104" t="n">
         <v>0.71</v>
@@ -2203,13 +2203,13 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>43</v>
+        <v>43.23895508379863</v>
       </c>
       <c r="B105" t="n">
-        <v>4.222700000000003</v>
+        <v>3.983744916201377</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D105" t="n">
         <v>0.71</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>43.22706991666667</v>
+        <v>43.33238899502331</v>
       </c>
       <c r="B106" t="n">
-        <v>3.995630083333333</v>
+        <v>3.890311004976697</v>
       </c>
       <c r="C106" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D106" t="n">
         <v>0.71</v>
@@ -2237,13 +2237,13 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>43.24431712534897</v>
+        <v>43.30484769444445</v>
       </c>
       <c r="B107" t="n">
-        <v>3.978382874651033</v>
+        <v>3.917852305555555</v>
       </c>
       <c r="C107" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D107" t="n">
         <v>0.71</v>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>43.27648937465104</v>
+        <v>43.1884175049767</v>
       </c>
       <c r="B108" t="n">
-        <v>3.946210625348967</v>
+        <v>4.034282495023302</v>
       </c>
       <c r="C108" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D108" t="n">
         <v>0.71</v>
@@ -2271,13 +2271,13 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>43.29373658333333</v>
+        <v>43</v>
       </c>
       <c r="B109" t="n">
-        <v>3.928963416666666</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C109" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
         <v>0.71</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>43</v>
+        <v>43.28185141620138</v>
       </c>
       <c r="B110" t="n">
-        <v>4.222700000000003</v>
+        <v>3.940848583798622</v>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D110" t="n">
         <v>0.71</v>
@@ -2305,13 +2305,13 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>43.20641394123253</v>
+        <v>43.26040325</v>
       </c>
       <c r="B111" t="n">
-        <v>4.016286058767476</v>
+        <v>3.96229675</v>
       </c>
       <c r="C111" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D111" t="n">
         <v>0.71</v>
@@ -2322,13 +2322,13 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>43.26040325</v>
+        <v>43</v>
       </c>
       <c r="B112" t="n">
-        <v>3.96229675</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C112" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
         <v>0.71</v>
@@ -2339,13 +2339,13 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>43.31439255876748</v>
+        <v>43</v>
       </c>
       <c r="B113" t="n">
-        <v>3.908307441232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C113" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D113" t="n">
         <v>0.71</v>
@@ -2356,13 +2356,13 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>43</v>
+        <v>43.21595880555556</v>
       </c>
       <c r="B114" t="n">
-        <v>4.222700000000003</v>
+        <v>4.006741194444444</v>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D114" t="n">
         <v>0.71</v>
@@ -2373,13 +2373,13 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>43</v>
+        <v>43.23895508379863</v>
       </c>
       <c r="B115" t="n">
-        <v>4.222700000000003</v>
+        <v>3.983744916201377</v>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D115" t="n">
         <v>0.71</v>
@@ -2390,13 +2390,13 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>43.22706991666667</v>
+        <v>43.33238899502331</v>
       </c>
       <c r="B116" t="n">
-        <v>3.995630083333333</v>
+        <v>3.890311004976697</v>
       </c>
       <c r="C116" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D116" t="n">
         <v>0.71</v>
@@ -2407,13 +2407,13 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>43.24431712534897</v>
+        <v>43.30484769444445</v>
       </c>
       <c r="B117" t="n">
-        <v>3.978382874651033</v>
+        <v>3.917852305555555</v>
       </c>
       <c r="C117" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D117" t="n">
         <v>0.71</v>
@@ -2424,13 +2424,13 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>43.27648937465104</v>
+        <v>43.1884175049767</v>
       </c>
       <c r="B118" t="n">
-        <v>3.946210625348967</v>
+        <v>4.034282495023302</v>
       </c>
       <c r="C118" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D118" t="n">
         <v>0.71</v>
@@ -2441,13 +2441,13 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>43.29373658333333</v>
+        <v>43</v>
       </c>
       <c r="B119" t="n">
-        <v>3.928963416666666</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C119" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D119" t="n">
         <v>0.71</v>
@@ -2458,13 +2458,13 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>43</v>
+        <v>43.28185141620138</v>
       </c>
       <c r="B120" t="n">
-        <v>4.222700000000003</v>
+        <v>3.940848583798622</v>
       </c>
       <c r="C120" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D120" t="n">
         <v>0.71</v>
@@ -2475,13 +2475,13 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>43.20641394123253</v>
+        <v>43.26040325</v>
       </c>
       <c r="B121" t="n">
-        <v>4.016286058767476</v>
+        <v>3.96229675</v>
       </c>
       <c r="C121" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D121" t="n">
         <v>0.71</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>43.27190311098868</v>
+        <v>43</v>
       </c>
       <c r="B123" t="n">
-        <v>3.950796889011324</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C123" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
         <v>0.7</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>43.20182767757017</v>
+        <v>43.23436882013627</v>
       </c>
       <c r="B124" t="n">
-        <v>4.020872322429834</v>
+        <v>3.988331179863735</v>
       </c>
       <c r="C124" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D124" t="n">
         <v>0.7</v>
@@ -2543,13 +2543,13 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>43</v>
+        <v>43.18383124131434</v>
       </c>
       <c r="B125" t="n">
-        <v>4.222700000000003</v>
+        <v>4.03886875868566</v>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D125" t="n">
         <v>0.7</v>
@@ -2560,13 +2560,13 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>43.22248365300431</v>
+        <v>43</v>
       </c>
       <c r="B126" t="n">
-        <v>4.000216346995691</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C126" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
         <v>0.7</v>
@@ -2577,13 +2577,13 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>43.28915031967098</v>
+        <v>43.25581698633765</v>
       </c>
       <c r="B127" t="n">
-        <v>3.933549680329024</v>
+        <v>3.966883013662357</v>
       </c>
       <c r="C127" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D127" t="n">
         <v>0.7</v>
@@ -2594,13 +2594,13 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>43.30980629510513</v>
+        <v>43.2113725418932</v>
       </c>
       <c r="B128" t="n">
-        <v>3.91289370489488</v>
+        <v>4.011327458106802</v>
       </c>
       <c r="C128" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D128" t="n">
         <v>0.7</v>
@@ -2611,13 +2611,13 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>43.23973086168661</v>
+        <v>43.27726515253902</v>
       </c>
       <c r="B129" t="n">
-        <v>3.98296913831339</v>
+        <v>3.94543484746098</v>
       </c>
       <c r="C129" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D129" t="n">
         <v>0.7</v>
@@ -2628,13 +2628,13 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>43</v>
+        <v>43.30026143078209</v>
       </c>
       <c r="B130" t="n">
-        <v>4.222700000000003</v>
+        <v>3.922438569217913</v>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D130" t="n">
         <v>0.7</v>
@@ -2645,13 +2645,13 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>43.25581698633765</v>
+        <v>43.32780273136095</v>
       </c>
       <c r="B131" t="n">
-        <v>3.966883013662357</v>
+        <v>3.894897268639055</v>
       </c>
       <c r="C131" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D131" t="n">
         <v>0.7</v>
@@ -2679,13 +2679,13 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>43.27190311098868</v>
+        <v>43</v>
       </c>
       <c r="B133" t="n">
-        <v>3.950796889011324</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C133" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D133" t="n">
         <v>0.7</v>
@@ -2696,13 +2696,13 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>43.20182767757017</v>
+        <v>43.23436882013627</v>
       </c>
       <c r="B134" t="n">
-        <v>4.020872322429834</v>
+        <v>3.988331179863735</v>
       </c>
       <c r="C134" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D134" t="n">
         <v>0.7</v>
@@ -2713,13 +2713,13 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>43</v>
+        <v>43.18383124131434</v>
       </c>
       <c r="B135" t="n">
-        <v>4.222700000000003</v>
+        <v>4.03886875868566</v>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D135" t="n">
         <v>0.7</v>
@@ -2730,13 +2730,13 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>43.22248365300431</v>
+        <v>43</v>
       </c>
       <c r="B136" t="n">
-        <v>4.000216346995691</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C136" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
         <v>0.7</v>
@@ -2747,13 +2747,13 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>43.28915031967098</v>
+        <v>43.25581698633765</v>
       </c>
       <c r="B137" t="n">
-        <v>3.933549680329024</v>
+        <v>3.966883013662357</v>
       </c>
       <c r="C137" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D137" t="n">
         <v>0.7</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>43.30980629510513</v>
+        <v>43.2113725418932</v>
       </c>
       <c r="B138" t="n">
-        <v>3.91289370489488</v>
+        <v>4.011327458106802</v>
       </c>
       <c r="C138" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D138" t="n">
         <v>0.7</v>
@@ -2781,13 +2781,13 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>43.23973086168661</v>
+        <v>43.27726515253902</v>
       </c>
       <c r="B139" t="n">
-        <v>3.98296913831339</v>
+        <v>3.94543484746098</v>
       </c>
       <c r="C139" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D139" t="n">
         <v>0.7</v>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>43</v>
+        <v>43.30026143078209</v>
       </c>
       <c r="B140" t="n">
-        <v>4.222700000000003</v>
+        <v>3.922438569217913</v>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D140" t="n">
         <v>0.7</v>
@@ -2815,13 +2815,13 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>43.25581698633765</v>
+        <v>43.32780273136095</v>
       </c>
       <c r="B141" t="n">
-        <v>3.966883013662357</v>
+        <v>3.894897268639055</v>
       </c>
       <c r="C141" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D141" t="n">
         <v>0.7</v>
@@ -2832,13 +2832,13 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>43.27688472624284</v>
+        <v>43.31553713793281</v>
       </c>
       <c r="B142" t="n">
-        <v>3.945815273757163</v>
+        <v>3.907162862067194</v>
       </c>
       <c r="C142" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D142" t="n">
         <v>0.6899999999999999</v>
@@ -2849,13 +2849,13 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>43</v>
+        <v>43.1715656478862</v>
       </c>
       <c r="B143" t="n">
-        <v>4.222700000000003</v>
+        <v>4.051134352113799</v>
       </c>
       <c r="C143" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D143" t="n">
         <v>0.6899999999999999</v>
@@ -2883,13 +2883,13 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>43.21021805957617</v>
+        <v>43.24355139290951</v>
       </c>
       <c r="B145" t="n">
-        <v>4.01248194042383</v>
+        <v>3.979148607090496</v>
       </c>
       <c r="C145" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D145" t="n">
         <v>0.6899999999999999</v>
@@ -2900,13 +2900,13 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>43.25963751756054</v>
+        <v>43.22210322670813</v>
       </c>
       <c r="B146" t="n">
-        <v>3.963062482439463</v>
+        <v>4.000596773291874</v>
       </c>
       <c r="C146" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D146" t="n">
         <v>0.6899999999999999</v>
@@ -2934,13 +2934,13 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>43.29754070167699</v>
+        <v>43.26499955911088</v>
       </c>
       <c r="B148" t="n">
-        <v>3.925159298323019</v>
+        <v>3.957700440889119</v>
       </c>
       <c r="C148" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D148" t="n">
         <v>0.6899999999999999</v>
@@ -2951,13 +2951,13 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>43.18956208414203</v>
+        <v>43.19910694846507</v>
       </c>
       <c r="B149" t="n">
-        <v>4.033137915857973</v>
+        <v>4.023593051534941</v>
       </c>
       <c r="C149" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D149" t="n">
         <v>0.6899999999999999</v>
@@ -2968,13 +2968,13 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>43.22746526825847</v>
+        <v>43</v>
       </c>
       <c r="B150" t="n">
-        <v>3.99523473174153</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C150" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D150" t="n">
         <v>0.6899999999999999</v>
@@ -2985,13 +2985,13 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>43.24355139290951</v>
+        <v>43.28799583735395</v>
       </c>
       <c r="B151" t="n">
-        <v>3.979148607090496</v>
+        <v>3.934704162646052</v>
       </c>
       <c r="C151" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D151" t="n">
         <v>0.6899999999999999</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>43.27688472624284</v>
+        <v>43.31553713793281</v>
       </c>
       <c r="B152" t="n">
-        <v>3.945815273757163</v>
+        <v>3.907162862067194</v>
       </c>
       <c r="C152" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D152" t="n">
         <v>0.6899999999999999</v>
@@ -3019,13 +3019,13 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>43</v>
+        <v>43.1715656478862</v>
       </c>
       <c r="B153" t="n">
-        <v>4.222700000000003</v>
+        <v>4.051134352113799</v>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D153" t="n">
         <v>0.6899999999999999</v>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>43.21021805957617</v>
+        <v>43.24355139290951</v>
       </c>
       <c r="B155" t="n">
-        <v>4.01248194042383</v>
+        <v>3.979148607090496</v>
       </c>
       <c r="C155" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D155" t="n">
         <v>0.6899999999999999</v>
@@ -3070,13 +3070,13 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>43.25963751756054</v>
+        <v>43.22210322670813</v>
       </c>
       <c r="B156" t="n">
-        <v>3.963062482439463</v>
+        <v>4.000596773291874</v>
       </c>
       <c r="C156" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D156" t="n">
         <v>0.6899999999999999</v>
@@ -3104,13 +3104,13 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>43.29754070167699</v>
+        <v>43.26499955911088</v>
       </c>
       <c r="B158" t="n">
-        <v>3.925159298323019</v>
+        <v>3.957700440889119</v>
       </c>
       <c r="C158" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D158" t="n">
         <v>0.6899999999999999</v>
@@ -3121,13 +3121,13 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>43.18956208414203</v>
+        <v>43.19910694846507</v>
       </c>
       <c r="B159" t="n">
-        <v>4.033137915857973</v>
+        <v>4.023593051534941</v>
       </c>
       <c r="C159" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D159" t="n">
         <v>0.6899999999999999</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>43.22746526825847</v>
+        <v>43</v>
       </c>
       <c r="B160" t="n">
-        <v>3.99523473174153</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C160" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D160" t="n">
         <v>0.6899999999999999</v>
@@ -3155,13 +3155,13 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>43.24355139290951</v>
+        <v>43.28799583735395</v>
       </c>
       <c r="B161" t="n">
-        <v>3.979148607090496</v>
+        <v>3.934704162646052</v>
       </c>
       <c r="C161" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D161" t="n">
         <v>0.6899999999999999</v>
@@ -3172,13 +3172,13 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>43.26162484284628</v>
+        <v>43</v>
       </c>
       <c r="B162" t="n">
-        <v>3.961075157153719</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C162" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D162" t="n">
         <v>0.6799999999999999</v>
@@ -3189,13 +3189,13 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>43.28228081828043</v>
+        <v>43.24973967571433</v>
       </c>
       <c r="B163" t="n">
-        <v>3.940419181719575</v>
+        <v>3.972960324285675</v>
       </c>
       <c r="C163" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D163" t="n">
         <v>0.6799999999999999</v>
@@ -3206,13 +3206,13 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>43.24437763416398</v>
+        <v>43.30027725453625</v>
       </c>
       <c r="B164" t="n">
-        <v>3.978322365836019</v>
+        <v>3.92242274546375</v>
       </c>
       <c r="C164" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D164" t="n">
         <v>0.6799999999999999</v>
@@ -3223,13 +3223,13 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>43.19495817617962</v>
+        <v>43</v>
       </c>
       <c r="B165" t="n">
-        <v>4.027741823820386</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C165" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D165" t="n">
         <v>0.6799999999999999</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>43</v>
+        <v>43.27273595395739</v>
       </c>
       <c r="B166" t="n">
-        <v>4.222700000000003</v>
+        <v>3.949964046042608</v>
       </c>
       <c r="C166" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D166" t="n">
         <v>0.6799999999999999</v>
@@ -3257,13 +3257,13 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>43.22829150951295</v>
+        <v>43</v>
       </c>
       <c r="B167" t="n">
-        <v>3.994408490487052</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C167" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D167" t="n">
         <v>0.6799999999999999</v>
@@ -3274,13 +3274,13 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>43.17430220074547</v>
+        <v>43.18384706506851</v>
       </c>
       <c r="B168" t="n">
-        <v>4.048397799254529</v>
+        <v>4.038852934931497</v>
       </c>
       <c r="C168" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D168" t="n">
         <v>0.6799999999999999</v>
@@ -3291,13 +3291,13 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>43</v>
+        <v>43.15630576448964</v>
       </c>
       <c r="B169" t="n">
-        <v>4.222700000000003</v>
+        <v>4.066394235510355</v>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D169" t="n">
         <v>0.6799999999999999</v>
@@ -3308,13 +3308,13 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>43.21220538486192</v>
+        <v>43.22829150951295</v>
       </c>
       <c r="B170" t="n">
-        <v>4.010494615138086</v>
+        <v>3.994408490487052</v>
       </c>
       <c r="C170" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D170" t="n">
         <v>0.6799999999999999</v>
@@ -3325,13 +3325,13 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>43</v>
+        <v>43.20684334331158</v>
       </c>
       <c r="B171" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01585665668843</v>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D171" t="n">
         <v>0.6799999999999999</v>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>43.26162484284628</v>
+        <v>43</v>
       </c>
       <c r="B172" t="n">
-        <v>3.961075157153719</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C172" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D172" t="n">
         <v>0.6799999999999999</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>43.28228081828043</v>
+        <v>43.24973967571433</v>
       </c>
       <c r="B173" t="n">
-        <v>3.940419181719575</v>
+        <v>3.972960324285675</v>
       </c>
       <c r="C173" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D173" t="n">
         <v>0.6799999999999999</v>
@@ -3376,13 +3376,13 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>43.24437763416398</v>
+        <v>43.30027725453625</v>
       </c>
       <c r="B174" t="n">
-        <v>3.978322365836019</v>
+        <v>3.92242274546375</v>
       </c>
       <c r="C174" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D174" t="n">
         <v>0.6799999999999999</v>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>43.19495817617962</v>
+        <v>43</v>
       </c>
       <c r="B175" t="n">
-        <v>4.027741823820386</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C175" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D175" t="n">
         <v>0.6799999999999999</v>
@@ -3410,13 +3410,13 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>43</v>
+        <v>43.27273595395739</v>
       </c>
       <c r="B176" t="n">
-        <v>4.222700000000003</v>
+        <v>3.949964046042608</v>
       </c>
       <c r="C176" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D176" t="n">
         <v>0.6799999999999999</v>
@@ -3427,13 +3427,13 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>43.22829150951295</v>
+        <v>43</v>
       </c>
       <c r="B177" t="n">
-        <v>3.994408490487052</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C177" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D177" t="n">
         <v>0.6799999999999999</v>
@@ -3444,13 +3444,13 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>43.17430220074547</v>
+        <v>43.18384706506851</v>
       </c>
       <c r="B178" t="n">
-        <v>4.048397799254529</v>
+        <v>4.038852934931497</v>
       </c>
       <c r="C178" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D178" t="n">
         <v>0.6799999999999999</v>
@@ -3461,13 +3461,13 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>43</v>
+        <v>43.15630576448964</v>
       </c>
       <c r="B179" t="n">
-        <v>4.222700000000003</v>
+        <v>4.066394235510355</v>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D179" t="n">
         <v>0.6799999999999999</v>
@@ -3478,13 +3478,13 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>43.21220538486192</v>
+        <v>43.22829150951295</v>
       </c>
       <c r="B180" t="n">
-        <v>4.010494615138086</v>
+        <v>3.994408490487052</v>
       </c>
       <c r="C180" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D180" t="n">
         <v>0.6799999999999999</v>
@@ -3495,13 +3495,13 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>43</v>
+        <v>43.20684334331158</v>
       </c>
       <c r="B181" t="n">
-        <v>4.222700000000003</v>
+        <v>4.01585665668843</v>
       </c>
       <c r="C181" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D181" t="n">
         <v>0.6799999999999999</v>
@@ -3512,13 +3512,13 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>43.23195221759212</v>
+        <v>43.19441792673971</v>
       </c>
       <c r="B182" t="n">
-        <v>3.990747782407881</v>
+        <v>4.028282073260291</v>
       </c>
       <c r="C182" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D182" t="n">
         <v>0.6699999999999999</v>
@@ -3529,13 +3529,13 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>43.16187678417361</v>
+        <v>43.28785183796439</v>
       </c>
       <c r="B183" t="n">
-        <v>4.060823215826391</v>
+        <v>3.934848162035611</v>
       </c>
       <c r="C183" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D183" t="n">
         <v>0.6699999999999999</v>
@@ -3546,13 +3546,13 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>43.24919942627442</v>
+        <v>43.17142164849665</v>
       </c>
       <c r="B184" t="n">
-        <v>3.97350057372558</v>
+        <v>4.051278351503358</v>
       </c>
       <c r="C184" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D184" t="n">
         <v>0.6699999999999999</v>
@@ -3563,13 +3563,13 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>43</v>
+        <v>43.23731425914247</v>
       </c>
       <c r="B185" t="n">
-        <v>4.222700000000003</v>
+        <v>3.985385740857536</v>
       </c>
       <c r="C185" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D185" t="n">
         <v>0.6699999999999999</v>
@@ -3580,13 +3580,13 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>43</v>
+        <v>43.21586609294109</v>
       </c>
       <c r="B186" t="n">
-        <v>4.222700000000003</v>
+        <v>4.006833907058914</v>
       </c>
       <c r="C186" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D186" t="n">
         <v>0.6699999999999999</v>
@@ -3597,13 +3597,13 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>43</v>
+        <v>43.26031053738554</v>
       </c>
       <c r="B187" t="n">
-        <v>4.222700000000003</v>
+        <v>3.962389462614469</v>
       </c>
       <c r="C187" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D187" t="n">
         <v>0.6699999999999999</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>43.18253275960775</v>
+        <v>43</v>
       </c>
       <c r="B188" t="n">
-        <v>4.040167240392247</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C188" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D188" t="n">
         <v>0.6699999999999999</v>
@@ -3631,13 +3631,13 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>43.19977996829006</v>
+        <v>43</v>
       </c>
       <c r="B189" t="n">
-        <v>4.022920031709947</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C189" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D189" t="n">
         <v>0.6699999999999999</v>
@@ -3648,13 +3648,13 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>43.26985540170857</v>
+        <v>43.14388034791779</v>
       </c>
       <c r="B190" t="n">
-        <v>3.952844598291437</v>
+        <v>4.078819652082216</v>
       </c>
       <c r="C190" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D190" t="n">
         <v>0.6699999999999999</v>
@@ -3665,13 +3665,13 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>43.21586609294109</v>
+        <v>43</v>
       </c>
       <c r="B191" t="n">
-        <v>4.006833907058914</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C191" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D191" t="n">
         <v>0.6699999999999999</v>
@@ -3682,13 +3682,13 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>43.23195221759212</v>
+        <v>43.19441792673971</v>
       </c>
       <c r="B192" t="n">
-        <v>3.990747782407881</v>
+        <v>4.028282073260291</v>
       </c>
       <c r="C192" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D192" t="n">
         <v>0.6699999999999999</v>
@@ -3699,13 +3699,13 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>43.16187678417361</v>
+        <v>43.28785183796439</v>
       </c>
       <c r="B193" t="n">
-        <v>4.060823215826391</v>
+        <v>3.934848162035611</v>
       </c>
       <c r="C193" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D193" t="n">
         <v>0.6699999999999999</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>43.24919942627442</v>
+        <v>43.17142164849665</v>
       </c>
       <c r="B194" t="n">
-        <v>3.97350057372558</v>
+        <v>4.051278351503358</v>
       </c>
       <c r="C194" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D194" t="n">
         <v>0.6699999999999999</v>
@@ -3733,13 +3733,13 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>43</v>
+        <v>43.23731425914247</v>
       </c>
       <c r="B195" t="n">
-        <v>4.222700000000003</v>
+        <v>3.985385740857536</v>
       </c>
       <c r="C195" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D195" t="n">
         <v>0.6699999999999999</v>
@@ -3750,13 +3750,13 @@
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>43</v>
+        <v>43.21586609294109</v>
       </c>
       <c r="B196" t="n">
-        <v>4.222700000000003</v>
+        <v>4.006833907058914</v>
       </c>
       <c r="C196" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D196" t="n">
         <v>0.6699999999999999</v>
@@ -3767,13 +3767,13 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>43</v>
+        <v>43.26031053738554</v>
       </c>
       <c r="B197" t="n">
-        <v>4.222700000000003</v>
+        <v>3.962389462614469</v>
       </c>
       <c r="C197" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D197" t="n">
         <v>0.6699999999999999</v>
@@ -3784,13 +3784,13 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>43.18253275960775</v>
+        <v>43</v>
       </c>
       <c r="B198" t="n">
-        <v>4.040167240392247</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C198" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D198" t="n">
         <v>0.6699999999999999</v>
@@ -3801,13 +3801,13 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>43.19977996829006</v>
+        <v>43</v>
       </c>
       <c r="B199" t="n">
-        <v>4.022920031709947</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C199" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D199" t="n">
         <v>0.6699999999999999</v>
@@ -3818,13 +3818,13 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>43.26985540170857</v>
+        <v>43.14388034791779</v>
       </c>
       <c r="B200" t="n">
-        <v>3.952844598291437</v>
+        <v>4.078819652082216</v>
       </c>
       <c r="C200" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D200" t="n">
         <v>0.6699999999999999</v>
@@ -3835,13 +3835,13 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>43.21586609294109</v>
+        <v>43</v>
       </c>
       <c r="B201" t="n">
-        <v>4.006833907058914</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C201" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D201" t="n">
         <v>0.6699999999999999</v>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>43.17768789666667</v>
+        <v>43.16657678555556</v>
       </c>
       <c r="B202" t="n">
-        <v>4.045012103333333</v>
+        <v>4.056123214444444</v>
       </c>
       <c r="C202" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D202" t="n">
         <v>0.6599999999999999</v>
@@ -3869,13 +3869,13 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>43</v>
+        <v>43.1390354849767</v>
       </c>
       <c r="B203" t="n">
-        <v>4.222700000000003</v>
+        <v>4.083664515023302</v>
       </c>
       <c r="C203" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D203" t="n">
         <v>0.6599999999999999</v>
@@ -3886,13 +3886,13 @@
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>43.24435456333334</v>
+        <v>43</v>
       </c>
       <c r="B204" t="n">
-        <v>3.978345436666666</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C204" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D204" t="n">
         <v>0.6599999999999999</v>
@@ -3903,13 +3903,13 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>43.26501053876748</v>
+        <v>43</v>
       </c>
       <c r="B205" t="n">
-        <v>3.957689461232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C205" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D205" t="n">
         <v>0.6599999999999999</v>
@@ -3920,13 +3920,13 @@
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>43</v>
+        <v>43.23246939620138</v>
       </c>
       <c r="B206" t="n">
-        <v>4.222700000000003</v>
+        <v>3.990230603798622</v>
       </c>
       <c r="C206" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D206" t="n">
         <v>0.6599999999999999</v>
@@ -3937,13 +3937,13 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>43.15703192123253</v>
+        <v>43.25546567444445</v>
       </c>
       <c r="B207" t="n">
-        <v>4.065668078767477</v>
+        <v>3.967234325555555</v>
       </c>
       <c r="C207" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D207" t="n">
         <v>0.6599999999999999</v>
@@ -3971,13 +3971,13 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>43.19493510534897</v>
+        <v>43.21102123</v>
       </c>
       <c r="B209" t="n">
-        <v>4.027764894651033</v>
+        <v>4.01167877</v>
       </c>
       <c r="C209" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D209" t="n">
         <v>0.6599999999999999</v>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>43.22710735465104</v>
+        <v>43.18957306379863</v>
       </c>
       <c r="B210" t="n">
-        <v>3.995592645348967</v>
+        <v>4.033126936201377</v>
       </c>
       <c r="C210" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D210" t="n">
         <v>0.6599999999999999</v>
@@ -4005,13 +4005,13 @@
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>43.21102123</v>
+        <v>43.28300697502331</v>
       </c>
       <c r="B211" t="n">
-        <v>4.01167877</v>
+        <v>3.939693024976697</v>
       </c>
       <c r="C211" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D211" t="n">
         <v>0.6599999999999999</v>
@@ -4022,13 +4022,13 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>43.17768789666667</v>
+        <v>43.16657678555556</v>
       </c>
       <c r="B212" t="n">
-        <v>4.045012103333333</v>
+        <v>4.056123214444444</v>
       </c>
       <c r="C212" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D212" t="n">
         <v>0.6599999999999999</v>
@@ -4039,13 +4039,13 @@
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>43</v>
+        <v>43.1390354849767</v>
       </c>
       <c r="B213" t="n">
-        <v>4.222700000000003</v>
+        <v>4.083664515023302</v>
       </c>
       <c r="C213" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D213" t="n">
         <v>0.6599999999999999</v>
@@ -4056,13 +4056,13 @@
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>43.24435456333334</v>
+        <v>43</v>
       </c>
       <c r="B214" t="n">
-        <v>3.978345436666666</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C214" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D214" t="n">
         <v>0.6599999999999999</v>
@@ -4073,13 +4073,13 @@
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>43.26501053876748</v>
+        <v>43</v>
       </c>
       <c r="B215" t="n">
-        <v>3.957689461232523</v>
+        <v>4.222700000000003</v>
       </c>
       <c r="C215" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D215" t="n">
         <v>0.6599999999999999</v>
@@ -4090,13 +4090,13 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>43</v>
+        <v>43.23246939620138</v>
       </c>
       <c r="B216" t="n">
-        <v>4.222700000000003</v>
+        <v>3.990230603798622</v>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D216" t="n">
         <v>0.6599999999999999</v>
@@ -4107,13 +4107,13 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>43.15703192123253</v>
+        <v>43.25546567444445</v>
       </c>
       <c r="B217" t="n">
-        <v>4.065668078767477</v>
+        <v>3.967234325555555</v>
       </c>
       <c r="C217" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D217" t="n">
         <v>0.6599999999999999</v>
@@ -4141,13 +4141,13 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>43.19493510534897</v>
+        <v>43.21102123</v>
       </c>
       <c r="B219" t="n">
-        <v>4.027764894651033</v>
+        <v>4.01167877</v>
       </c>
       <c r="C219" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D219" t="n">
         <v>0.6599999999999999</v>
@@ -4158,13 +4158,13 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>43.22710735465104</v>
+        <v>43.18957306379863</v>
       </c>
       <c r="B220" t="n">
-        <v>3.995592645348967</v>
+        <v>4.033126936201377</v>
       </c>
       <c r="C220" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D220" t="n">
         <v>0.6599999999999999</v>
@@ -4175,13 +4175,13 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>43.21102123</v>
+        <v>43.28300697502331</v>
       </c>
       <c r="B221" t="n">
-        <v>4.01167877</v>
+        <v>3.939693024976697</v>
       </c>
       <c r="C221" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D221" t="n">
         <v>0.6599999999999999</v>

</xml_diff>

<commit_message>
implementing C(T/TF) correction for DC HFT
</commit_message>
<xml_diff>
--- a/phase_shift_scanlist.xlsx
+++ b/phase_shift_scanlist.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,1906 +462,2144 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B2" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E2" t="n">
-        <v>0.28</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B3" t="n">
-        <v>47.37340719586602</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C3" t="n">
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="E3" t="n">
-        <v>0.28</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>202.0816090522714</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B4" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C4" t="n">
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="E4" t="n">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>202.2419585285108</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B5" t="n">
-        <v>47.3899773894429</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C5" t="n">
         <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>0.71</v>
+        <v>0.49</v>
       </c>
       <c r="E5" t="n">
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B6" t="n">
-        <v>47.38374582059588</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="E6" t="n">
-        <v>0.27</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B7" t="n">
-        <v>47.38374582059588</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E7" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>202.0816090522714</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B8" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="E8" t="n">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>202.1443548738203</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B9" t="n">
-        <v>47.37340719586602</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>0.28</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>202.0443277736058</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B10" t="n">
-        <v>47.35642064920658</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.75</v>
+        <v>0.53</v>
       </c>
       <c r="E10" t="n">
-        <v>0.21</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B11" t="n">
-        <v>47.38374582059588</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E11" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>202.2419585285108</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B12" t="n">
-        <v>47.3899773894429</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.71</v>
+        <v>0.55</v>
       </c>
       <c r="E12" t="n">
-        <v>0.25</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B13" t="n">
-        <v>47.35642064920658</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.75</v>
+        <v>0.49</v>
       </c>
       <c r="E13" t="n">
-        <v>0.21</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>202.203751576025</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B14" t="n">
-        <v>47.38349155203341</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>0.72</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E14" t="n">
-        <v>0.24</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>202.1443548738203</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B15" t="n">
-        <v>47.37340719586602</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="E15" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>202.1443548738203</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B16" t="n">
-        <v>47.37340719586602</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C16" t="n">
         <v>10</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="E16" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>202.0816090522714</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B17" t="n">
-        <v>47.36275231806718</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.74</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>0.22</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>202.2419585285108</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B18" t="n">
-        <v>47.3899773894429</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.71</v>
+        <v>0.51</v>
       </c>
       <c r="E18" t="n">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>202.0443277736058</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B19" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C19" t="n">
         <v>10</v>
       </c>
       <c r="D19" t="n">
-        <v>0.75</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>0.21</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>202.0443277736058</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B20" t="n">
-        <v>47.35642064920658</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="E20" t="n">
-        <v>0.21</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>202.2419585285108</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B21" t="n">
-        <v>47.3899773894429</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.71</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B22" t="n">
-        <v>47.38374582059588</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="E22" t="n">
-        <v>0.27</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B23" t="n">
-        <v>47.39007450063703</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7</v>
+        <v>0.49</v>
       </c>
       <c r="E23" t="n">
-        <v>0.26</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>202.0816090522714</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B24" t="n">
-        <v>47.36275231806718</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.74</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E24" t="n">
-        <v>0.22</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>202.2419585285108</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B25" t="n">
-        <v>47.3899773894429</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="E25" t="n">
-        <v>0.25</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>202.203751576025</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B26" t="n">
-        <v>47.38349155203341</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D26" t="n">
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="E26" t="n">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>202.2419585285108</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B27" t="n">
-        <v>47.3899773894429</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.71</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E27" t="n">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B28" t="n">
-        <v>47.3730928463169</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28" t="n">
-        <v>0.73</v>
+        <v>0.51</v>
       </c>
       <c r="E28" t="n">
-        <v>0.23</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B29" t="n">
-        <v>47.35642064920658</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
-        <v>0.75</v>
+        <v>0.57</v>
       </c>
       <c r="E29" t="n">
-        <v>0.21</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B30" t="n">
-        <v>47.3730928463169</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
-        <v>0.73</v>
+        <v>0.49</v>
       </c>
       <c r="E30" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>202.0443277736058</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B31" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C31" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.75</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>0.21</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B32" t="n">
-        <v>47.39007450063703</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C32" t="n">
         <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>0.7</v>
+        <v>0.57</v>
       </c>
       <c r="E32" t="n">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>202.2052493477286</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B33" t="n">
-        <v>47.38374582059588</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C33" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="E33" t="n">
-        <v>0.27</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>202.203751576025</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B34" t="n">
-        <v>47.38349155203341</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D34" t="n">
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="E34" t="n">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>202.0816090522714</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B35" t="n">
-        <v>47.36275231806718</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C35" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0.74</v>
+        <v>0.55</v>
       </c>
       <c r="E35" t="n">
-        <v>0.22</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>202.203751576025</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B36" t="n">
-        <v>47.38349155203341</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C36" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.72</v>
+        <v>0.57</v>
       </c>
       <c r="E36" t="n">
-        <v>0.24</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B37" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C37" t="n">
         <v>10</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="E37" t="n">
-        <v>0.28</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>202.2419585285108</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B38" t="n">
-        <v>47.3899773894429</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C38" t="n">
         <v>10</v>
       </c>
       <c r="D38" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="E38" t="n">
-        <v>0.25</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B39" t="n">
-        <v>47.3730928463169</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C39" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.73</v>
+        <v>0.59</v>
       </c>
       <c r="E39" t="n">
-        <v>0.23</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>202.2052493477286</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B40" t="n">
-        <v>47.38374582059588</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C40" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="E40" t="n">
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>202.2425306263942</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B41" t="n">
-        <v>47.39007450063703</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7</v>
+        <v>0.53</v>
       </c>
       <c r="E41" t="n">
-        <v>0.26</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B42" t="n">
-        <v>47.39007450063703</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C42" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="E42" t="n">
-        <v>0.26</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B43" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C43" t="n">
         <v>10</v>
       </c>
       <c r="D43" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="E43" t="n">
-        <v>0.28</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B44" t="n">
-        <v>47.38374582059588</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E44" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>202.1443548738203</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B45" t="n">
-        <v>47.37340719586602</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C45" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E45" t="n">
-        <v>0.28</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B46" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="E46" t="n">
-        <v>0.28</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B47" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C47" t="n">
         <v>10</v>
       </c>
       <c r="D47" t="n">
-        <v>0.75</v>
+        <v>0.59</v>
       </c>
       <c r="E47" t="n">
-        <v>0.21</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B48" t="n">
-        <v>47.39007450063703</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.7</v>
+        <v>0.59</v>
       </c>
       <c r="E48" t="n">
-        <v>0.26</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>202.0816090522714</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B49" t="n">
-        <v>47.36275231806718</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D49" t="n">
-        <v>0.74</v>
+        <v>0.49</v>
       </c>
       <c r="E49" t="n">
-        <v>0.22</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>202.203751576025</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B50" t="n">
-        <v>47.38349155203341</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C50" t="n">
         <v>10</v>
       </c>
       <c r="D50" t="n">
-        <v>0.72</v>
+        <v>0.53</v>
       </c>
       <c r="E50" t="n">
-        <v>0.24</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>202.203751576025</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B51" t="n">
-        <v>47.38349155203341</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C51" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.72</v>
+        <v>0.57</v>
       </c>
       <c r="E51" t="n">
-        <v>0.24</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B52" t="n">
-        <v>47.39007450063703</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C52" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7</v>
+        <v>0.59</v>
       </c>
       <c r="E52" t="n">
-        <v>0.26</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>202.1425035261798</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B53" t="n">
-        <v>47.3730928463169</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C53" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.73</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E53" t="n">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>202.0816090522714</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B54" t="n">
-        <v>47.36275231806718</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.74</v>
+        <v>0.53</v>
       </c>
       <c r="E54" t="n">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>202.203751576025</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B55" t="n">
-        <v>47.38349155203341</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="E55" t="n">
-        <v>0.24</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>202.0443277736058</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B56" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.75</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E56" t="n">
-        <v>0.21</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>202.2419585285108</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B57" t="n">
-        <v>47.3899773894429</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.71</v>
+        <v>0.61</v>
       </c>
       <c r="E57" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>202.1425035261798</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B58" t="n">
-        <v>47.3730928463169</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C58" t="n">
         <v>10</v>
       </c>
       <c r="D58" t="n">
-        <v>0.73</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E58" t="n">
-        <v>0.23</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>202.2419585285108</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B59" t="n">
-        <v>47.3899773894429</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.71</v>
+        <v>0.59</v>
       </c>
       <c r="E59" t="n">
-        <v>0.25</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B60" t="n">
-        <v>47.3730928463169</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C60" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.73</v>
+        <v>0.57</v>
       </c>
       <c r="E60" t="n">
-        <v>0.23</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>202.203751576025</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B61" t="n">
-        <v>47.38349155203341</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.72</v>
+        <v>0.53</v>
       </c>
       <c r="E61" t="n">
-        <v>0.24</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>202.1443548738203</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B62" t="n">
-        <v>47.37340719586602</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="E62" t="n">
-        <v>0.28</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>202.203751576025</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B63" t="n">
-        <v>47.38349155203341</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C63" t="n">
         <v>10</v>
       </c>
       <c r="D63" t="n">
-        <v>0.72</v>
+        <v>0.55</v>
       </c>
       <c r="E63" t="n">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>202.2419585285108</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B64" t="n">
-        <v>47.3899773894429</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C64" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.71</v>
+        <v>0.53</v>
       </c>
       <c r="E64" t="n">
-        <v>0.25</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B65" t="n">
-        <v>47.38374582059588</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D65" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="E65" t="n">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>202.1425035261798</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B66" t="n">
-        <v>47.3730928463169</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C66" t="n">
         <v>10</v>
       </c>
       <c r="D66" t="n">
-        <v>0.73</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E66" t="n">
-        <v>0.23</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>202.2052493477286</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B67" t="n">
-        <v>47.38374582059588</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D67" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="E67" t="n">
-        <v>0.27</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B68" t="n">
-        <v>47.37340719586602</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C68" t="n">
         <v>10</v>
       </c>
       <c r="D68" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="E68" t="n">
-        <v>0.28</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>202.203751576025</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B69" t="n">
-        <v>47.38349155203341</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C69" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0.72</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E69" t="n">
-        <v>0.24</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B70" t="n">
-        <v>47.38374582059588</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C70" t="n">
         <v>10</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E70" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>202.2419585285108</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B71" t="n">
-        <v>47.3899773894429</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.71</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E71" t="n">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>202.2425306263942</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B72" t="n">
-        <v>47.39007450063703</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C72" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="E72" t="n">
-        <v>0.26</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B73" t="n">
-        <v>47.35642064920658</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>0.75</v>
+        <v>0.49</v>
       </c>
       <c r="E73" t="n">
-        <v>0.21</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>202.2425306263942</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B74" t="n">
-        <v>47.39007450063703</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C74" t="n">
         <v>10</v>
       </c>
       <c r="D74" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="E74" t="n">
-        <v>0.26</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>202.2419585285108</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B75" t="n">
-        <v>47.3899773894429</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.71</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E75" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>202.0443277736058</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B76" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D76" t="n">
-        <v>0.75</v>
+        <v>0.61</v>
       </c>
       <c r="E76" t="n">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B77" t="n">
-        <v>47.39007450063703</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C77" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>0.7</v>
+        <v>0.49</v>
       </c>
       <c r="E77" t="n">
-        <v>0.26</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>202.2052493477286</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B78" t="n">
-        <v>47.38374582059588</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.57</v>
       </c>
       <c r="E78" t="n">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>202.0816090522714</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B79" t="n">
-        <v>47.36275231806718</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C79" t="n">
         <v>10</v>
       </c>
       <c r="D79" t="n">
-        <v>0.74</v>
+        <v>0.53</v>
       </c>
       <c r="E79" t="n">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>202.2419585285108</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B80" t="n">
-        <v>47.3899773894429</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C80" t="n">
         <v>10</v>
       </c>
       <c r="D80" t="n">
-        <v>0.71</v>
+        <v>0.51</v>
       </c>
       <c r="E80" t="n">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>202.1443548738203</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B81" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E81" t="n">
-        <v>0.28</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>202.2425306263942</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B82" t="n">
-        <v>47.39007450063703</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>0.7</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E82" t="n">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>202.1443548738203</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B83" t="n">
-        <v>47.37340719586602</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D83" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="E83" t="n">
-        <v>0.28</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>202.2052493477286</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B84" t="n">
-        <v>47.38374582059588</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C84" t="n">
         <v>10</v>
       </c>
       <c r="D84" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="E84" t="n">
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>202.0443277736058</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B85" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C85" t="n">
         <v>10</v>
       </c>
       <c r="D85" t="n">
-        <v>0.75</v>
+        <v>0.61</v>
       </c>
       <c r="E85" t="n">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>202.2052493477286</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B86" t="n">
-        <v>47.38374582059588</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C86" t="n">
         <v>10</v>
       </c>
       <c r="D86" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E86" t="n">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>202.2425306263942</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B87" t="n">
-        <v>47.39007450063703</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C87" t="n">
         <v>10</v>
       </c>
       <c r="D87" t="n">
-        <v>0.7</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E87" t="n">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B88" t="n">
-        <v>47.35642064920658</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C88" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0.75</v>
+        <v>0.59</v>
       </c>
       <c r="E88" t="n">
-        <v>0.21</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>202.1425035261798</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B89" t="n">
-        <v>47.3730928463169</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>0.73</v>
+        <v>0.61</v>
       </c>
       <c r="E89" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>202.0816090522714</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B90" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C90" t="n">
         <v>10</v>
       </c>
       <c r="D90" t="n">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="E90" t="n">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>202.0443277736058</v>
+        <v>202.128818436632</v>
       </c>
       <c r="B91" t="n">
-        <v>47.35642064920658</v>
+        <v>47.37076913374894</v>
       </c>
       <c r="C91" t="n">
         <v>10</v>
       </c>
       <c r="D91" t="n">
-        <v>0.75</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="E91" t="n">
-        <v>0.21</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>202.1443548738203</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B92" t="n">
-        <v>47.37340719586602</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C92" t="n">
         <v>10</v>
       </c>
       <c r="D92" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="E92" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>202.203751576025</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B93" t="n">
-        <v>47.38349155203341</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D93" t="n">
-        <v>0.72</v>
+        <v>0.57</v>
       </c>
       <c r="E93" t="n">
-        <v>0.24</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>202.2419585285108</v>
+        <v>202.1654549711855</v>
       </c>
       <c r="B94" t="n">
-        <v>47.3899773894429</v>
+        <v>47.37698976600116</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D94" t="n">
-        <v>0.71</v>
+        <v>0.57</v>
       </c>
       <c r="E94" t="n">
-        <v>0.25</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>202.1425035261798</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B95" t="n">
-        <v>47.3730928463169</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C95" t="n">
         <v>10</v>
       </c>
       <c r="D95" t="n">
-        <v>0.73</v>
+        <v>0.53</v>
       </c>
       <c r="E95" t="n">
-        <v>0.23</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>202.1425035261798</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B96" t="n">
-        <v>47.3730928463169</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0.73</v>
+        <v>0.61</v>
       </c>
       <c r="E96" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>202.0816090522714</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B97" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D97" t="n">
-        <v>0.74</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E97" t="n">
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>202.1425035261798</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B98" t="n">
-        <v>47.3730928463169</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D98" t="n">
-        <v>0.73</v>
+        <v>0.55</v>
       </c>
       <c r="E98" t="n">
-        <v>0.23</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>202.203751576025</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B99" t="n">
-        <v>47.38349155203341</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C99" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.72</v>
+        <v>0.51</v>
       </c>
       <c r="E99" t="n">
-        <v>0.24</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>202.0816090522714</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B100" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C100" t="n">
         <v>10</v>
       </c>
       <c r="D100" t="n">
-        <v>0.74</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E100" t="n">
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B101" t="n">
-        <v>47.39007450063703</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="E101" t="n">
-        <v>0.26</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>202.0816090522714</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B102" t="n">
-        <v>47.36275231806718</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D102" t="n">
-        <v>0.74</v>
+        <v>0.53</v>
       </c>
       <c r="E102" t="n">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B103" t="n">
-        <v>47.3730928463169</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D103" t="n">
-        <v>0.73</v>
+        <v>0.51</v>
       </c>
       <c r="E103" t="n">
-        <v>0.23</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>202.2425306263942</v>
+        <v>202.1916135448988</v>
       </c>
       <c r="B104" t="n">
-        <v>47.39007450063703</v>
+        <v>47.38143090323386</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D104" t="n">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="E104" t="n">
-        <v>0.26</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1174710690708</v>
       </c>
       <c r="B105" t="n">
-        <v>47.3730928463169</v>
+        <v>47.36884229294331</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D105" t="n">
-        <v>0.73</v>
+        <v>0.59</v>
       </c>
       <c r="E105" t="n">
-        <v>0.23</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>202.0816090522714</v>
+        <v>202.0877254268452</v>
       </c>
       <c r="B106" t="n">
-        <v>47.36275231806718</v>
+        <v>47.36379102688297</v>
       </c>
       <c r="C106" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="E106" t="n">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>202.2425306263942</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B107" t="n">
-        <v>47.39007450063703</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D107" t="n">
-        <v>0.7</v>
+        <v>0.53</v>
       </c>
       <c r="E107" t="n">
-        <v>0.26</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>202.203751576025</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B108" t="n">
-        <v>47.38349155203341</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C108" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>0.72</v>
+        <v>0.55</v>
       </c>
       <c r="E108" t="n">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>202.1425035261798</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B109" t="n">
-        <v>47.3730928463169</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C109" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.73</v>
+        <v>0.49</v>
       </c>
       <c r="E109" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>202.2052493477286</v>
+        <v>202.09234204899</v>
       </c>
       <c r="B110" t="n">
-        <v>47.38374582059588</v>
+        <v>47.36457502899982</v>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D110" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="E110" t="n">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>202.0816090522714</v>
+        <v>202.2163093379161</v>
       </c>
       <c r="B111" t="n">
-        <v>47.36275231806718</v>
+        <v>47.3856233804354</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D111" t="n">
-        <v>0.74</v>
+        <v>0.53</v>
       </c>
       <c r="E111" t="n">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>202.0443277736058</v>
+        <v>202.1449661377905</v>
       </c>
       <c r="B112" t="n">
-        <v>47.35642064920658</v>
+        <v>47.37351098504899</v>
       </c>
       <c r="C112" t="n">
         <v>10</v>
       </c>
       <c r="D112" t="n">
-        <v>0.75</v>
+        <v>0.49</v>
       </c>
       <c r="E112" t="n">
-        <v>0.21</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>202.203751576025</v>
+        <v>202.2056668474857</v>
       </c>
       <c r="B113" t="n">
-        <v>47.38349155203341</v>
+        <v>47.38381669706164</v>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D113" t="n">
-        <v>0.72</v>
+        <v>0.55</v>
       </c>
       <c r="E113" t="n">
-        <v>0.24</v>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>202.1916135448988</v>
+      </c>
+      <c r="B114" t="n">
+        <v>47.38143090323386</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>202.1174710690708</v>
+      </c>
+      <c r="B115" t="n">
+        <v>47.36884229294331</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>202.128818436632</v>
+      </c>
+      <c r="B116" t="n">
+        <v>47.37076913374894</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>202.128818436632</v>
+      </c>
+      <c r="B117" t="n">
+        <v>47.37076913374894</v>
+      </c>
+      <c r="C117" t="n">
+        <v>10</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>202.128818436632</v>
+      </c>
+      <c r="B118" t="n">
+        <v>47.37076913374894</v>
+      </c>
+      <c r="C118" t="n">
+        <v>10</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>202.2163093379161</v>
+      </c>
+      <c r="B119" t="n">
+        <v>47.3856233804354</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>202.1174710690708</v>
+      </c>
+      <c r="B120" t="n">
+        <v>47.36884229294331</v>
+      </c>
+      <c r="C120" t="n">
+        <v>10</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>202.1654549711855</v>
+      </c>
+      <c r="B121" t="n">
+        <v>47.37698976600116</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>202.1916135448988</v>
+      </c>
+      <c r="B122" t="n">
+        <v>47.38143090323386</v>
+      </c>
+      <c r="C122" t="n">
+        <v>10</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>202.1916135448988</v>
+      </c>
+      <c r="B123" t="n">
+        <v>47.38143090323386</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>202.1174710690708</v>
+      </c>
+      <c r="B124" t="n">
+        <v>47.36884229294331</v>
+      </c>
+      <c r="C124" t="n">
+        <v>10</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>202.1449661377905</v>
+      </c>
+      <c r="B125" t="n">
+        <v>47.37351098504899</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>202.128818436632</v>
+      </c>
+      <c r="B126" t="n">
+        <v>47.37076913374894</v>
+      </c>
+      <c r="C126" t="n">
+        <v>10</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>202.0877254268452</v>
+      </c>
+      <c r="B127" t="n">
+        <v>47.36379102688297</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>